<commit_message>
Finished ANA1 without gigazine
</commit_message>
<xml_diff>
--- a/Netbeans/ANA-ADDIX/input/input - Copy.xlsx
+++ b/Netbeans/ANA-ADDIX/input/input - Copy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\Sources\11. ChangeCodeANA\ANA-VIETNAM\Netbeans\ANA-ADDIX\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\Sources\11. ChangeCodeANA\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA67B8C-0197-451C-AD60-3BD3C2A6287C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69589BF7-BFA3-4710-93DE-114E11C4E840}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1449,7 +1449,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="4">
         <v>1</v>
@@ -1647,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>

</xml_diff>